<commit_message>
1. Vocabs refactored.  2. Model generation enhanced to handle multiple specialisations.
</commit_message>
<xml_diff>
--- a/templates/citations.xlsx
+++ b/templates/citations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a-0/Engineering/ipsl/esdoc/repos/cordex/cordexp/lib/citations/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a-0/Engineering/ipsl/esdoc/repos/cordex/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC6F94C-1E9F-0B4C-B2D2-E53992AC0125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F20B3A-15CD-9E40-B32D-53A49802906B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="460" windowWidth="33040" windowHeight="19120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6400" yWindow="2340" windowWidth="33040" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -70,10 +70,10 @@
     <t>Long name for internal use (unarchived)</t>
   </si>
   <si>
-    <t>ES-DOC CORDEXP Model Citations</t>
+    <t>ES-DOC CORDEX Model Citations</t>
   </si>
   <si>
-    <t>CORDEXP Model Citations</t>
+    <t>CORDEX Model Citations</t>
   </si>
 </sst>
 </file>
@@ -1529,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2288,7 +2288,7 @@
   </sheetPr>
   <dimension ref="A1:IP52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>